<commit_message>
add sectoral distribution of labor plots
</commit_message>
<xml_diff>
--- a/datasets/labor/labor_sectoral_haryana.xlsx
+++ b/datasets/labor/labor_sectoral_haryana.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\econ_gju\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\econ_gju\datasets\labor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342BCB8B-FD3B-4D02-AE21-D3E00ABA384F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D16FC0-3350-4F18-9C99-39FC39C1DAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="19">
   <si>
     <t>Age</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Rural+Urban</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Primary Sector</t>
   </si>
   <si>
@@ -85,18 +82,6 @@
   </si>
   <si>
     <t>Tertiary Sector</t>
-  </si>
-  <si>
-    <t>Primary Sector (%)</t>
-  </si>
-  <si>
-    <t>Secondary Sector (%)</t>
-  </si>
-  <si>
-    <t>Tertiary Sector (%)</t>
-  </si>
-  <si>
-    <t>Total (%)</t>
   </si>
 </sst>
 </file>
@@ -125,18 +110,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -157,21 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -488,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="E2:G2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -503,15 +472,10 @@
     <col min="5" max="5" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,32 +488,17 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -571,23 +520,8 @@
       <c r="G2" s="1">
         <v>30.08</v>
       </c>
-      <c r="H2" s="1">
-        <v>100</v>
-      </c>
-      <c r="I2" s="3">
-        <v>336102.65222379565</v>
-      </c>
-      <c r="J2" s="3">
-        <v>449335.0965558766</v>
-      </c>
-      <c r="K2" s="3">
-        <v>337899.99261001917</v>
-      </c>
-      <c r="L2" s="3">
-        <v>1123337.7413896914</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -609,23 +543,8 @@
       <c r="G3" s="1">
         <v>68.33</v>
       </c>
-      <c r="H3" s="1">
-        <v>100</v>
-      </c>
-      <c r="I3" s="3">
-        <v>40496.891574525296</v>
-      </c>
-      <c r="J3" s="3">
-        <v>23662.01568736646</v>
-      </c>
-      <c r="K3" s="3">
-        <v>138426.84348610873</v>
-      </c>
-      <c r="L3" s="3">
-        <v>202585.75074800052</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -647,23 +566,8 @@
       <c r="G4" s="1">
         <v>33.47</v>
       </c>
-      <c r="H4" s="1">
-        <v>100</v>
-      </c>
-      <c r="I4" s="3">
-        <v>402068.29782957601</v>
-      </c>
-      <c r="J4" s="3">
-        <v>519061.31148866407</v>
-      </c>
-      <c r="K4" s="3">
-        <v>463403.09670647071</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1384532.7060247108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,23 +589,8 @@
       <c r="G5" s="1">
         <v>53.21</v>
       </c>
-      <c r="H5" s="1">
-        <v>100</v>
-      </c>
-      <c r="I5" s="3">
-        <v>15873.724559588632</v>
-      </c>
-      <c r="J5" s="3">
-        <v>426228.40171609714</v>
-      </c>
-      <c r="K5" s="3">
-        <v>502762.43084268528</v>
-      </c>
-      <c r="L5" s="3">
-        <v>944864.55711837101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -723,23 +612,8 @@
       <c r="G6" s="1">
         <v>65.430000000000007</v>
       </c>
-      <c r="H6" s="1">
-        <v>100</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>36095.798072862293</v>
-      </c>
-      <c r="K6" s="3">
-        <v>68317.849809296487</v>
-      </c>
-      <c r="L6" s="3">
-        <v>104413.64788215878</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -761,23 +635,8 @@
       <c r="G7" s="1">
         <v>55.25</v>
       </c>
-      <c r="H7" s="1">
-        <v>100</v>
-      </c>
-      <c r="I7" s="3">
-        <v>14267.996112107983</v>
-      </c>
-      <c r="J7" s="3">
-        <v>441798.30818562937</v>
-      </c>
-      <c r="K7" s="3">
-        <v>563076.27513854729</v>
-      </c>
-      <c r="L7" s="3">
-        <v>1019142.5794362846</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -799,23 +658,8 @@
       <c r="G8" s="1">
         <v>38.81</v>
       </c>
-      <c r="H8" s="1">
-        <v>100</v>
-      </c>
-      <c r="I8" s="3">
-        <v>394477.78827967006</v>
-      </c>
-      <c r="J8" s="3">
-        <v>858798.2171633729</v>
-      </c>
-      <c r="K8" s="3">
-        <v>794895.2732676008</v>
-      </c>
-      <c r="L8" s="3">
-        <v>2048171.2787106438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -837,23 +681,8 @@
       <c r="G9" s="1">
         <v>66.72</v>
       </c>
-      <c r="H9" s="1">
-        <v>100</v>
-      </c>
-      <c r="I9" s="3">
-        <v>27447.177654914354</v>
-      </c>
-      <c r="J9" s="3">
-        <v>75302.211811401692</v>
-      </c>
-      <c r="K9" s="3">
-        <v>205992.76638198938</v>
-      </c>
-      <c r="L9" s="3">
-        <v>308742.15584830544</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -875,23 +704,8 @@
       <c r="G10" s="1">
         <v>42.15</v>
       </c>
-      <c r="H10" s="1">
-        <v>100</v>
-      </c>
-      <c r="I10" s="3">
-        <v>431813.23522665218</v>
-      </c>
-      <c r="J10" s="3">
-        <v>954446.23524292768</v>
-      </c>
-      <c r="K10" s="3">
-        <v>1010040.3920534622</v>
-      </c>
-      <c r="L10" s="3">
-        <v>2396299.8625230421</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -913,23 +727,8 @@
       <c r="G11" s="1">
         <v>32.5</v>
       </c>
-      <c r="H11" s="1">
-        <v>100</v>
-      </c>
-      <c r="I11" s="3">
-        <v>308713.04434678628</v>
-      </c>
-      <c r="J11" s="3">
-        <v>529506.20317566243</v>
-      </c>
-      <c r="K11" s="3">
-        <v>403587.04510340118</v>
-      </c>
-      <c r="L11" s="3">
-        <v>1241806.2926258498</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -951,23 +750,8 @@
       <c r="G12" s="1">
         <v>28.63</v>
       </c>
-      <c r="H12" s="1">
-        <v>100</v>
-      </c>
-      <c r="I12" s="3">
-        <v>68588.56808831291</v>
-      </c>
-      <c r="J12" s="3">
-        <v>26629.601615302967</v>
-      </c>
-      <c r="K12" s="3">
-        <v>38196.668048403</v>
-      </c>
-      <c r="L12" s="3">
-        <v>133414.83775201888</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -989,23 +773,8 @@
       <c r="G13" s="1">
         <v>32.11</v>
       </c>
-      <c r="H13" s="1">
-        <v>100</v>
-      </c>
-      <c r="I13" s="3">
-        <v>375306.86811220134</v>
-      </c>
-      <c r="J13" s="3">
-        <v>550886.63520067942</v>
-      </c>
-      <c r="K13" s="3">
-        <v>438062.6512207482</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1364256.1545336288</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1027,23 +796,8 @@
       <c r="G14" s="1">
         <v>43.89</v>
       </c>
-      <c r="H14" s="1">
-        <v>100</v>
-      </c>
-      <c r="I14" s="3">
-        <v>40242.757619886681</v>
-      </c>
-      <c r="J14" s="3">
-        <v>478842.5596334103</v>
-      </c>
-      <c r="K14" s="3">
-        <v>406035.54757168429</v>
-      </c>
-      <c r="L14" s="3">
-        <v>925120.8648249812</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1065,23 +819,8 @@
       <c r="G15" s="1">
         <v>85.99</v>
       </c>
-      <c r="H15" s="1">
-        <v>100</v>
-      </c>
-      <c r="I15" s="3">
-        <v>1908.9041843552245</v>
-      </c>
-      <c r="J15" s="3">
-        <v>22871.500134774629</v>
-      </c>
-      <c r="K15" s="3">
-        <v>151987.65815991271</v>
-      </c>
-      <c r="L15" s="3">
-        <v>176750.38744029854</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1103,23 +842,8 @@
       <c r="G16" s="1">
         <v>50.55</v>
       </c>
-      <c r="H16" s="1">
-        <v>100</v>
-      </c>
-      <c r="I16" s="3">
-        <v>42353.574118609045</v>
-      </c>
-      <c r="J16" s="3">
-        <v>504483.04211251816</v>
-      </c>
-      <c r="K16" s="3">
-        <v>559000.82811897842</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1105837.4443501057</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1141,23 +865,8 @@
       <c r="G17" s="1">
         <v>36.57</v>
       </c>
-      <c r="H17" s="1">
-        <v>100</v>
-      </c>
-      <c r="I17" s="3">
-        <v>377049.96144816739</v>
-      </c>
-      <c r="J17" s="3">
-        <v>986692.88657188637</v>
-      </c>
-      <c r="K17" s="3">
-        <v>786129.82270008465</v>
-      </c>
-      <c r="L17" s="3">
-        <v>2149657.7049496435</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1179,23 +888,8 @@
       <c r="G18" s="1">
         <v>56.45</v>
       </c>
-      <c r="H18" s="1">
-        <v>100</v>
-      </c>
-      <c r="I18" s="3">
-        <v>78934.693260887012</v>
-      </c>
-      <c r="J18" s="3">
-        <v>48384.043461765934</v>
-      </c>
-      <c r="K18" s="3">
-        <v>165031.97905841007</v>
-      </c>
-      <c r="L18" s="3">
-        <v>292350.71578106302</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1217,23 +911,8 @@
       <c r="G19" s="1">
         <v>38.979999999999997</v>
       </c>
-      <c r="H19" s="1">
-        <v>100</v>
-      </c>
-      <c r="I19" s="3">
-        <v>454222.74705113622</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1028745.2585700692</v>
-      </c>
-      <c r="K19" s="3">
-        <v>947330.26645549957</v>
-      </c>
-      <c r="L19" s="3">
-        <v>2430298.272076705</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1255,23 +934,8 @@
       <c r="G20" s="1">
         <v>38.130000000000003</v>
       </c>
-      <c r="H20" s="1">
-        <v>100</v>
-      </c>
-      <c r="I20" s="3">
-        <v>299419.51562734466</v>
-      </c>
-      <c r="J20" s="3">
-        <v>492250.80197367305</v>
-      </c>
-      <c r="K20" s="3">
-        <v>487900.26200301939</v>
-      </c>
-      <c r="L20" s="3">
-        <v>1279570.5796040371</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1293,23 +957,8 @@
       <c r="G21" s="1">
         <v>19.04</v>
       </c>
-      <c r="H21" s="1">
-        <v>100</v>
-      </c>
-      <c r="I21" s="3">
-        <v>97483.162261366058</v>
-      </c>
-      <c r="J21" s="3">
-        <v>12298.960658096956</v>
-      </c>
-      <c r="K21" s="3">
-        <v>25818.325350624698</v>
-      </c>
-      <c r="L21" s="3">
-        <v>135600.44827008771</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1331,23 +980,8 @@
       <c r="G22" s="1">
         <v>35.520000000000003</v>
       </c>
-      <c r="H22" s="1">
-        <v>100</v>
-      </c>
-      <c r="I22" s="3">
-        <v>420165.08373813139</v>
-      </c>
-      <c r="J22" s="3">
-        <v>481707.23981162591</v>
-      </c>
-      <c r="K22" s="3">
-        <v>496813.04175693833</v>
-      </c>
-      <c r="L22" s="3">
-        <v>1398685.3653066957</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1369,23 +1003,8 @@
       <c r="G23" s="1">
         <v>44.86</v>
       </c>
-      <c r="H23" s="1">
-        <v>100</v>
-      </c>
-      <c r="I23" s="3">
-        <v>4974.9071692667139</v>
-      </c>
-      <c r="J23" s="3">
-        <v>512509.30460747652</v>
-      </c>
-      <c r="K23" s="3">
-        <v>421083.65210057504</v>
-      </c>
-      <c r="L23" s="3">
-        <v>938661.7300503233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1407,23 +1026,8 @@
       <c r="G24" s="1">
         <v>40.92</v>
       </c>
-      <c r="H24" s="1">
-        <v>100</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0</v>
-      </c>
-      <c r="J24" s="3">
-        <v>113033.02818899654</v>
-      </c>
-      <c r="K24" s="3">
-        <v>78288.955881749134</v>
-      </c>
-      <c r="L24" s="3">
-        <v>191321.98407074568</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1445,23 +1049,8 @@
       <c r="G25" s="1">
         <v>44.45</v>
       </c>
-      <c r="H25" s="1">
-        <v>100</v>
-      </c>
-      <c r="I25" s="3">
-        <v>5336.5868190001183</v>
-      </c>
-      <c r="J25" s="3">
-        <v>625402.55742665217</v>
-      </c>
-      <c r="K25" s="3">
-        <v>504704.85979692615</v>
-      </c>
-      <c r="L25" s="3">
-        <v>1135444.0040425784</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1483,23 +1072,8 @@
       <c r="G26" s="1">
         <v>40.65</v>
       </c>
-      <c r="H26" s="1">
-        <v>100</v>
-      </c>
-      <c r="I26" s="3">
-        <v>328064.17113078432</v>
-      </c>
-      <c r="J26" s="3">
-        <v>983971.44589159102</v>
-      </c>
-      <c r="K26" s="3">
-        <v>898639.39059746522</v>
-      </c>
-      <c r="L26" s="3">
-        <v>2210675.0076198406</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1521,23 +1095,8 @@
       <c r="G27" s="1">
         <v>25.81</v>
       </c>
-      <c r="H27" s="1">
-        <v>100</v>
-      </c>
-      <c r="I27" s="3">
-        <v>155247.88748351994</v>
-      </c>
-      <c r="J27" s="3">
-        <v>76717.341096366887</v>
-      </c>
-      <c r="K27" s="3">
-        <v>80687.635439984908</v>
-      </c>
-      <c r="L27" s="3">
-        <v>312621.60185968579</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1559,23 +1118,8 @@
       <c r="G28" s="1">
         <v>38.79</v>
       </c>
-      <c r="H28" s="1">
-        <v>100</v>
-      </c>
-      <c r="I28" s="3">
-        <v>482316.34166544088</v>
-      </c>
-      <c r="J28" s="3">
-        <v>1053969.1129005472</v>
-      </c>
-      <c r="K28" s="3">
-        <v>973415.75927171973</v>
-      </c>
-      <c r="L28" s="3">
-        <v>2509450.2688108268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1597,23 +1141,8 @@
       <c r="G29" s="1">
         <v>26.71</v>
       </c>
-      <c r="H29" s="1">
-        <v>100</v>
-      </c>
-      <c r="I29" s="3">
-        <v>1783697.9302180409</v>
-      </c>
-      <c r="J29" s="3">
-        <v>1431785.0790409518</v>
-      </c>
-      <c r="K29" s="3">
-        <v>1172018.9844064915</v>
-      </c>
-      <c r="L29" s="3">
-        <v>4387940.7877442585</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -1635,23 +1164,8 @@
       <c r="G30" s="1">
         <v>27.36</v>
       </c>
-      <c r="H30" s="1">
-        <v>100</v>
-      </c>
-      <c r="I30" s="3">
-        <v>523501.01362740737</v>
-      </c>
-      <c r="J30" s="3">
-        <v>57686.723341794393</v>
-      </c>
-      <c r="K30" s="3">
-        <v>218905.51326373019</v>
-      </c>
-      <c r="L30" s="3">
-        <v>800093.25023293192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -1673,23 +1187,8 @@
       <c r="G31" s="1">
         <v>26.81</v>
       </c>
-      <c r="H31" s="1">
-        <v>100</v>
-      </c>
-      <c r="I31" s="3">
-        <v>2298378.5456098025</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1503165.5392078576</v>
-      </c>
-      <c r="K31" s="3">
-        <v>1392531.7244700296</v>
-      </c>
-      <c r="L31" s="3">
-        <v>5194075.8092876896</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1711,23 +1210,8 @@
       <c r="G32" s="1">
         <v>52.86</v>
       </c>
-      <c r="H32" s="1">
-        <v>100</v>
-      </c>
-      <c r="I32" s="3">
-        <v>137097.53262421934</v>
-      </c>
-      <c r="J32" s="3">
-        <v>1394366.3744624394</v>
-      </c>
-      <c r="K32" s="3">
-        <v>1717292.790169724</v>
-      </c>
-      <c r="L32" s="3">
-        <v>3248756.6972563826</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
@@ -1749,23 +1233,8 @@
       <c r="G33" s="1">
         <v>63.74</v>
       </c>
-      <c r="H33" s="1">
-        <v>100</v>
-      </c>
-      <c r="I33" s="3">
-        <v>28562.598442146733</v>
-      </c>
-      <c r="J33" s="3">
-        <v>144050.70480989336</v>
-      </c>
-      <c r="K33" s="3">
-        <v>303430.00411707209</v>
-      </c>
-      <c r="L33" s="3">
-        <v>476043.30736911215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
@@ -1787,23 +1256,8 @@
       <c r="G34" s="1">
         <v>54.9</v>
       </c>
-      <c r="H34" s="1">
-        <v>100</v>
-      </c>
-      <c r="I34" s="3">
-        <v>164958.86696739023</v>
-      </c>
-      <c r="J34" s="3">
-        <v>1470127.9242917963</v>
-      </c>
-      <c r="K34" s="3">
-        <v>1990382.8124197193</v>
-      </c>
-      <c r="L34" s="3">
-        <v>3625469.6036789063</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
@@ -1825,23 +1279,8 @@
       <c r="G35" s="1">
         <v>36.409999999999997</v>
       </c>
-      <c r="H35" s="1">
-        <v>100</v>
-      </c>
-      <c r="I35" s="3">
-        <v>2067306.9087759636</v>
-      </c>
-      <c r="J35" s="3">
-        <v>2776467.8270038273</v>
-      </c>
-      <c r="K35" s="3">
-        <v>2773420.9487300231</v>
-      </c>
-      <c r="L35" s="3">
-        <v>7617195.6845098138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1863,23 +1302,8 @@
       <c r="G36" s="1">
         <v>43.54</v>
       </c>
-      <c r="H36" s="1">
-        <v>100</v>
-      </c>
-      <c r="I36" s="3">
-        <v>500108.56520817889</v>
-      </c>
-      <c r="J36" s="3">
-        <v>223894.75765473858</v>
-      </c>
-      <c r="K36" s="3">
-        <v>558326.33151702839</v>
-      </c>
-      <c r="L36" s="3">
-        <v>1282329.6543799459</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -1901,23 +1325,8 @@
       <c r="G37" s="1">
         <v>37.56</v>
       </c>
-      <c r="H37" s="1">
-        <v>100</v>
-      </c>
-      <c r="I37" s="3">
-        <v>2560718.4582431181</v>
-      </c>
-      <c r="J37" s="3">
-        <v>2943283.6254987163</v>
-      </c>
-      <c r="K37" s="3">
-        <v>3310863.5212258697</v>
-      </c>
-      <c r="L37" s="3">
-        <v>8814865.604967704</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
@@ -1939,23 +1348,8 @@
       <c r="G38" s="1">
         <v>32.94</v>
       </c>
-      <c r="H38" s="1">
-        <v>100</v>
-      </c>
-      <c r="I38" s="3">
-        <v>1549186.0709365231</v>
-      </c>
-      <c r="J38" s="3">
-        <v>1407228.7815678378</v>
-      </c>
-      <c r="K38" s="3">
-        <v>1452196.6185728249</v>
-      </c>
-      <c r="L38" s="3">
-        <v>4408611.4710771861</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -1977,23 +1371,8 @@
       <c r="G39" s="1">
         <v>24.46</v>
       </c>
-      <c r="H39" s="1">
-        <v>100</v>
-      </c>
-      <c r="I39" s="3">
-        <v>463642.30826864974</v>
-      </c>
-      <c r="J39" s="3">
-        <v>113903.8811739964</v>
-      </c>
-      <c r="K39" s="3">
-        <v>186985.83446415784</v>
-      </c>
-      <c r="L39" s="3">
-        <v>764455.57834896911</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -2015,23 +1394,8 @@
       <c r="G40" s="1">
         <v>31.66</v>
       </c>
-      <c r="H40" s="1">
-        <v>100</v>
-      </c>
-      <c r="I40" s="3">
-        <v>2002730.176291761</v>
-      </c>
-      <c r="J40" s="3">
-        <v>1507569.3940539416</v>
-      </c>
-      <c r="K40" s="3">
-        <v>1626223.0669760748</v>
-      </c>
-      <c r="L40" s="3">
-        <v>5136522.6373217776</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -2053,23 +1417,8 @@
       <c r="G41" s="1">
         <v>52.02</v>
       </c>
-      <c r="H41" s="1">
-        <v>100</v>
-      </c>
-      <c r="I41" s="3">
-        <v>154409.49106635747</v>
-      </c>
-      <c r="J41" s="3">
-        <v>1351396.8872596247</v>
-      </c>
-      <c r="K41" s="3">
-        <v>1632597.9116406334</v>
-      </c>
-      <c r="L41" s="3">
-        <v>3138404.2899666154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2091,23 +1440,8 @@
       <c r="G42" s="1">
         <v>73.05</v>
       </c>
-      <c r="H42" s="1">
-        <v>100</v>
-      </c>
-      <c r="I42" s="3">
-        <v>34512.642543387461</v>
-      </c>
-      <c r="J42" s="3">
-        <v>153010.68740505853</v>
-      </c>
-      <c r="K42" s="3">
-        <v>508296.07616823667</v>
-      </c>
-      <c r="L42" s="3">
-        <v>695819.40611668269</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -2129,23 +1463,8 @@
       <c r="G43" s="1">
         <v>55.79</v>
       </c>
-      <c r="H43" s="1">
-        <v>100</v>
-      </c>
-      <c r="I43" s="3">
-        <v>189641.50110297624</v>
-      </c>
-      <c r="J43" s="3">
-        <v>1510977.3150760459</v>
-      </c>
-      <c r="K43" s="3">
-        <v>2146064.776173437</v>
-      </c>
-      <c r="L43" s="3">
-        <v>3846683.5923524592</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2167,23 +1486,8 @@
       <c r="G44" s="1">
         <v>39.520000000000003</v>
       </c>
-      <c r="H44" s="1">
-        <v>100</v>
-      </c>
-      <c r="I44" s="3">
-        <v>1855659.7817533645</v>
-      </c>
-      <c r="J44" s="3">
-        <v>2686238.3809517543</v>
-      </c>
-      <c r="K44" s="3">
-        <v>2967854.0904448791</v>
-      </c>
-      <c r="L44" s="3">
-        <v>7509752.2531499974</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>11</v>
       </c>
@@ -2205,23 +1509,8 @@
       <c r="G45" s="1">
         <v>43.57</v>
       </c>
-      <c r="H45" s="1">
-        <v>100</v>
-      </c>
-      <c r="I45" s="3">
-        <v>550583.52548490418</v>
-      </c>
-      <c r="J45" s="3">
-        <v>251415.141090035</v>
-      </c>
-      <c r="K45" s="3">
-        <v>619228.81273560342</v>
-      </c>
-      <c r="L45" s="3">
-        <v>1421227.4793105426</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -2243,23 +1532,8 @@
       <c r="G46" s="1">
         <v>40.18</v>
       </c>
-      <c r="H46" s="1">
-        <v>100</v>
-      </c>
-      <c r="I46" s="3">
-        <v>2398815.1568599911</v>
-      </c>
-      <c r="J46" s="3">
-        <v>2922694.3290478056</v>
-      </c>
-      <c r="K46" s="3">
-        <v>3573763.1814102507</v>
-      </c>
-      <c r="L46" s="3">
-        <v>8894383.2289951481</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
@@ -2281,23 +1555,8 @@
       <c r="G47" s="1">
         <v>33.409999999999997</v>
       </c>
-      <c r="H47" s="1">
-        <v>100</v>
-      </c>
-      <c r="I47" s="3">
-        <v>1665669.9759164026</v>
-      </c>
-      <c r="J47" s="3">
-        <v>1384012.8312398596</v>
-      </c>
-      <c r="K47" s="3">
-        <v>1530108.1631940338</v>
-      </c>
-      <c r="L47" s="3">
-        <v>4579790.9703502962</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -2319,23 +1578,8 @@
       <c r="G48" s="1">
         <v>21.28</v>
       </c>
-      <c r="H48" s="1">
-        <v>100</v>
-      </c>
-      <c r="I48" s="3">
-        <v>518353.89459202217</v>
-      </c>
-      <c r="J48" s="3">
-        <v>99245.902324641764</v>
-      </c>
-      <c r="K48" s="3">
-        <v>166952.79062991121</v>
-      </c>
-      <c r="L48" s="3">
-        <v>784552.58754657512</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
@@ -2357,23 +1601,8 @@
       <c r="G49" s="1">
         <v>31.54</v>
       </c>
-      <c r="H49" s="1">
-        <v>100</v>
-      </c>
-      <c r="I49" s="3">
-        <v>2171744.9096586728</v>
-      </c>
-      <c r="J49" s="3">
-        <v>1458967.0931553135</v>
-      </c>
-      <c r="K49" s="3">
-        <v>1672694.3699788651</v>
-      </c>
-      <c r="L49" s="3">
-        <v>5303406.3727928512</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -2395,23 +1624,8 @@
       <c r="G50" s="1">
         <v>50.63</v>
       </c>
-      <c r="H50" s="1">
-        <v>100</v>
-      </c>
-      <c r="I50" s="3">
-        <v>89586.150593579485</v>
-      </c>
-      <c r="J50" s="3">
-        <v>1524599.3438608071</v>
-      </c>
-      <c r="K50" s="3">
-        <v>1655382.0454572735</v>
-      </c>
-      <c r="L50" s="3">
-        <v>3269567.5399116599</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>12</v>
       </c>
@@ -2433,23 +1647,8 @@
       <c r="G51" s="1">
         <v>56.52</v>
       </c>
-      <c r="H51" s="1">
-        <v>100</v>
-      </c>
-      <c r="I51" s="3">
-        <v>64854.65530681191</v>
-      </c>
-      <c r="J51" s="3">
-        <v>269573.79857066303</v>
-      </c>
-      <c r="K51" s="3">
-        <v>434826.22988624073</v>
-      </c>
-      <c r="L51" s="3">
-        <v>769331.61692540825</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>12</v>
       </c>
@@ -2471,23 +1670,8 @@
       <c r="G52" s="1">
         <v>51.43</v>
       </c>
-      <c r="H52" s="1">
-        <v>100</v>
-      </c>
-      <c r="I52" s="3">
-        <v>142181.91693155665</v>
-      </c>
-      <c r="J52" s="3">
-        <v>1825275.5489845993</v>
-      </c>
-      <c r="K52" s="3">
-        <v>2083309.3982307578</v>
-      </c>
-      <c r="L52" s="3">
-        <v>4050766.8641469139</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -2509,23 +1693,8 @@
       <c r="G53" s="1">
         <v>39.659999999999997</v>
       </c>
-      <c r="H53" s="1">
-        <v>100</v>
-      </c>
-      <c r="I53" s="3">
-        <v>1892193.718368168</v>
-      </c>
-      <c r="J53" s="3">
-        <v>2831636.1933544325</v>
-      </c>
-      <c r="K53" s="3">
-        <v>3104857.3798296042</v>
-      </c>
-      <c r="L53" s="3">
-        <v>7828687.2915522046</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
@@ -2547,23 +1716,8 @@
       <c r="G54" s="1">
         <v>32.869999999999997</v>
       </c>
-      <c r="H54" s="1">
-        <v>100</v>
-      </c>
-      <c r="I54" s="3">
-        <v>715370.13901028153</v>
-      </c>
-      <c r="J54" s="3">
-        <v>303789.39901518961</v>
-      </c>
-      <c r="K54" s="3">
-        <v>499028.3630999141</v>
-      </c>
-      <c r="L54" s="3">
-        <v>1518187.9011253854</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
@@ -2585,23 +1739,8 @@
       <c r="G55" s="1">
         <v>38.659999999999997</v>
       </c>
-      <c r="H55" s="1">
-        <v>100</v>
-      </c>
-      <c r="I55" s="3">
-        <v>2563075.1502617039</v>
-      </c>
-      <c r="J55" s="3">
-        <v>3142464.0539674521</v>
-      </c>
-      <c r="K55" s="3">
-        <v>3595373.196992652</v>
-      </c>
-      <c r="L55" s="3">
-        <v>9299982.4029815104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -2623,23 +1762,8 @@
       <c r="G56" s="1">
         <v>26.85</v>
       </c>
-      <c r="H56" s="1">
-        <v>100</v>
-      </c>
-      <c r="I56" s="3">
-        <v>1763460.1089995501</v>
-      </c>
-      <c r="J56" s="3">
-        <v>1415374.4640245282</v>
-      </c>
-      <c r="K56" s="3">
-        <v>1166803.9410211416</v>
-      </c>
-      <c r="L56" s="3">
-        <v>4345638.5140452199</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -2661,23 +1785,8 @@
       <c r="G57" s="1">
         <v>27.36</v>
       </c>
-      <c r="H57" s="1">
-        <v>100</v>
-      </c>
-      <c r="I57" s="3">
-        <v>510519.50458010333</v>
-      </c>
-      <c r="J57" s="3">
-        <v>56256.237628343944</v>
-      </c>
-      <c r="K57" s="3">
-        <v>213477.20686705832</v>
-      </c>
-      <c r="L57" s="3">
-        <v>780252.94907550549</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -2699,23 +1808,8 @@
       <c r="G58" s="1">
         <v>26.93</v>
       </c>
-      <c r="H58" s="1">
-        <v>100</v>
-      </c>
-      <c r="I58" s="3">
-        <v>2256313.0711071584</v>
-      </c>
-      <c r="J58" s="3">
-        <v>1475949.4738568782</v>
-      </c>
-      <c r="K58" s="3">
-        <v>1375339.7692375686</v>
-      </c>
-      <c r="L58" s="3">
-        <v>5107091.6050411016</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -2737,23 +1831,8 @@
       <c r="G59" s="1">
         <v>52.86</v>
       </c>
-      <c r="H59" s="1">
-        <v>100</v>
-      </c>
-      <c r="I59" s="3">
-        <v>129772.59396112018</v>
-      </c>
-      <c r="J59" s="3">
-        <v>1319867.235263336</v>
-      </c>
-      <c r="K59" s="3">
-        <v>1625540.1224608561</v>
-      </c>
-      <c r="L59" s="3">
-        <v>3075179.9516853122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -2775,23 +1854,8 @@
       <c r="G60" s="1">
         <v>63.7</v>
       </c>
-      <c r="H60" s="1">
-        <v>100</v>
-      </c>
-      <c r="I60" s="3">
-        <v>28487.44702671214</v>
-      </c>
-      <c r="J60" s="3">
-        <v>144149.33545570032</v>
-      </c>
-      <c r="K60" s="3">
-        <v>302946.64033415081</v>
-      </c>
-      <c r="L60" s="3">
-        <v>475583.42281656322</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -2813,23 +1877,8 @@
       <c r="G61" s="1">
         <v>54.89</v>
       </c>
-      <c r="H61" s="1">
-        <v>100</v>
-      </c>
-      <c r="I61" s="3">
-        <v>160326.38118306603</v>
-      </c>
-      <c r="J61" s="3">
-        <v>1429195.1694033316</v>
-      </c>
-      <c r="K61" s="3">
-        <v>1934135.1787117571</v>
-      </c>
-      <c r="L61" s="3">
-        <v>3523656.7292981548</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -2851,23 +1900,8 @@
       <c r="G62" s="1">
         <v>36.49</v>
       </c>
-      <c r="H62" s="1">
-        <v>100</v>
-      </c>
-      <c r="I62" s="3">
-        <v>2002558.1635538219</v>
-      </c>
-      <c r="J62" s="3">
-        <v>2689529.4258574191</v>
-      </c>
-      <c r="K62" s="3">
-        <v>2695438.8560707844</v>
-      </c>
-      <c r="L62" s="3">
-        <v>7386787.7667053547</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -2889,23 +1923,8 @@
       <c r="G63" s="1">
         <v>43.53</v>
       </c>
-      <c r="H63" s="1">
-        <v>100</v>
-      </c>
-      <c r="I63" s="3">
-        <v>490660.46627977083</v>
-      </c>
-      <c r="J63" s="3">
-        <v>220098.7831555063</v>
-      </c>
-      <c r="K63" s="3">
-        <v>547793.02634415042</v>
-      </c>
-      <c r="L63" s="3">
-        <v>1258426.4331361139</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -2927,23 +1946,8 @@
       <c r="G64" s="1">
         <v>37.619999999999997</v>
       </c>
-      <c r="H64" s="1">
-        <v>100</v>
-      </c>
-      <c r="I64" s="3">
-        <v>2495814.9535015486</v>
-      </c>
-      <c r="J64" s="3">
-        <v>2869069.1539907535</v>
-      </c>
-      <c r="K64" s="3">
-        <v>3235443.0927197887</v>
-      </c>
-      <c r="L64" s="3">
-        <v>8600327.2002120912</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>11</v>
       </c>
@@ -2965,23 +1969,8 @@
       <c r="G65" s="1">
         <v>32.94</v>
       </c>
-      <c r="H65" s="1">
-        <v>100</v>
-      </c>
-      <c r="I65" s="3">
-        <v>1549268.3738157945</v>
-      </c>
-      <c r="J65" s="3">
-        <v>1407303.5427490086</v>
-      </c>
-      <c r="K65" s="3">
-        <v>1452273.7687391085</v>
-      </c>
-      <c r="L65" s="3">
-        <v>4408845.6853039116</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>11</v>
       </c>
@@ -3003,23 +1992,8 @@
       <c r="G66" s="1">
         <v>24.46</v>
       </c>
-      <c r="H66" s="1">
-        <v>100</v>
-      </c>
-      <c r="I66" s="3">
-        <v>464448.6702152362</v>
-      </c>
-      <c r="J66" s="3">
-        <v>114101.98163572991</v>
-      </c>
-      <c r="K66" s="3">
-        <v>187311.03830939287</v>
-      </c>
-      <c r="L66" s="3">
-        <v>765785.11164919403</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>11</v>
       </c>
@@ -3041,23 +2015,8 @@
       <c r="G67" s="1">
         <v>31.66</v>
       </c>
-      <c r="H67" s="1">
-        <v>100</v>
-      </c>
-      <c r="I67" s="3">
-        <v>2003579.6779172975</v>
-      </c>
-      <c r="J67" s="3">
-        <v>1508208.8624486453</v>
-      </c>
-      <c r="K67" s="3">
-        <v>1626912.864910532</v>
-      </c>
-      <c r="L67" s="3">
-        <v>5138701.4052764745</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>11</v>
       </c>
@@ -3079,23 +2038,8 @@
       <c r="G68" s="1">
         <v>52.11</v>
       </c>
-      <c r="H68" s="1">
-        <v>100</v>
-      </c>
-      <c r="I68" s="3">
-        <v>154383.26413243817</v>
-      </c>
-      <c r="J68" s="3">
-        <v>1351089.3808087306</v>
-      </c>
-      <c r="K68" s="3">
-        <v>1638474.9274829638</v>
-      </c>
-      <c r="L68" s="3">
-        <v>3144261.9986239951</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>11</v>
       </c>
@@ -3117,23 +2061,8 @@
       <c r="G69" s="1">
         <v>73.05</v>
       </c>
-      <c r="H69" s="1">
-        <v>100</v>
-      </c>
-      <c r="I69" s="3">
-        <v>34516.893598924093</v>
-      </c>
-      <c r="J69" s="3">
-        <v>153029.53432264936</v>
-      </c>
-      <c r="K69" s="3">
-        <v>508358.68495996064</v>
-      </c>
-      <c r="L69" s="3">
-        <v>695905.11288153415</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>11</v>
       </c>
@@ -3155,23 +2084,8 @@
       <c r="G70" s="1">
         <v>55.86</v>
       </c>
-      <c r="H70" s="1">
-        <v>100</v>
-      </c>
-      <c r="I70" s="3">
-        <v>189581.11182115442</v>
-      </c>
-      <c r="J70" s="3">
-        <v>1511254.3100865197</v>
-      </c>
-      <c r="K70" s="3">
-        <v>2152439.2086035949</v>
-      </c>
-      <c r="L70" s="3">
-        <v>3853274.630511269</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -3193,23 +2107,8 @@
       <c r="G71" s="1">
         <v>39.57</v>
       </c>
-      <c r="H71" s="1">
-        <v>100</v>
-      </c>
-      <c r="I71" s="3">
-        <v>1855495.8637227747</v>
-      </c>
-      <c r="J71" s="3">
-        <v>2685922.3235906023</v>
-      </c>
-      <c r="K71" s="3">
-        <v>2973753.3952008989</v>
-      </c>
-      <c r="L71" s="3">
-        <v>7515171.5825142749</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>11</v>
       </c>
@@ -3231,23 +2130,8 @@
       <c r="G72" s="1">
         <v>43.57</v>
       </c>
-      <c r="H72" s="1">
-        <v>100</v>
-      </c>
-      <c r="I72" s="3">
-        <v>551002.00604530284</v>
-      </c>
-      <c r="J72" s="3">
-        <v>251606.23352972139</v>
-      </c>
-      <c r="K72" s="3">
-        <v>619699.4683374766</v>
-      </c>
-      <c r="L72" s="3">
-        <v>1422307.7079125007</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>11</v>
       </c>
@@ -3269,23 +2153,8 @@
       <c r="G73" s="1">
         <v>40.21</v>
       </c>
-      <c r="H73" s="1">
-        <v>100</v>
-      </c>
-      <c r="I73" s="3">
-        <v>2398941.2492421893</v>
-      </c>
-      <c r="J73" s="3">
-        <v>2923236.7578891842</v>
-      </c>
-      <c r="K73" s="3">
-        <v>3579273.7525799056</v>
-      </c>
-      <c r="L73" s="3">
-        <v>8901451.7597112786</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>12</v>
       </c>
@@ -3307,23 +2176,8 @@
       <c r="G74" s="1">
         <v>33.56</v>
       </c>
-      <c r="H74" s="1">
-        <v>100</v>
-      </c>
-      <c r="I74" s="3">
-        <v>1664335.1121087568</v>
-      </c>
-      <c r="J74" s="3">
-        <v>1383581.7800771804</v>
-      </c>
-      <c r="K74" s="3">
-        <v>1539555.8534280562</v>
-      </c>
-      <c r="L74" s="3">
-        <v>4587472.7456139931</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>12</v>
       </c>
@@ -3345,23 +2199,8 @@
       <c r="G75" s="1">
         <v>21.28</v>
       </c>
-      <c r="H75" s="1">
-        <v>100</v>
-      </c>
-      <c r="I75" s="3">
-        <v>519457.20004085876</v>
-      </c>
-      <c r="J75" s="3">
-        <v>99457.145156907296</v>
-      </c>
-      <c r="K75" s="3">
-        <v>167308.14616118476</v>
-      </c>
-      <c r="L75" s="3">
-        <v>786222.49135895085</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>12</v>
       </c>
@@ -3383,23 +2222,8 @@
       <c r="G76" s="1">
         <v>31.67</v>
       </c>
-      <c r="H76" s="1">
-        <v>100</v>
-      </c>
-      <c r="I76" s="3">
-        <v>2172900.3833453418</v>
-      </c>
-      <c r="J76" s="3">
-        <v>1460299.6702560717</v>
-      </c>
-      <c r="K76" s="3">
-        <v>1684183.9241445663</v>
-      </c>
-      <c r="L76" s="3">
-        <v>5317915.7693229122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>12</v>
       </c>
@@ -3421,23 +2245,8 @@
       <c r="G77" s="1">
         <v>50.64</v>
       </c>
-      <c r="H77" s="1">
-        <v>100</v>
-      </c>
-      <c r="I77" s="3">
-        <v>89217.961363259528</v>
-      </c>
-      <c r="J77" s="3">
-        <v>1523895.0689995578</v>
-      </c>
-      <c r="K77" s="3">
-        <v>1654944.1624305726</v>
-      </c>
-      <c r="L77" s="3">
-        <v>3268057.1927933898</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>12</v>
       </c>
@@ -3459,23 +2268,8 @@
       <c r="G78" s="1">
         <v>56.52</v>
       </c>
-      <c r="H78" s="1">
-        <v>100</v>
-      </c>
-      <c r="I78" s="3">
-        <v>64739.572921519401</v>
-      </c>
-      <c r="J78" s="3">
-        <v>269095.44901186711</v>
-      </c>
-      <c r="K78" s="3">
-        <v>434054.64549516921</v>
-      </c>
-      <c r="L78" s="3">
-        <v>767966.46407496324</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>12</v>
       </c>
@@ -3497,23 +2291,8 @@
       <c r="G79" s="1">
         <v>51.43</v>
       </c>
-      <c r="H79" s="1">
-        <v>100</v>
-      </c>
-      <c r="I79" s="3">
-        <v>142337.77167147322</v>
-      </c>
-      <c r="J79" s="3">
-        <v>1827276.3508594257</v>
-      </c>
-      <c r="K79" s="3">
-        <v>2085593.0475965438</v>
-      </c>
-      <c r="L79" s="3">
-        <v>4055207.1701274426</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>12</v>
       </c>
@@ -3535,23 +2314,8 @@
       <c r="G80" s="1">
         <v>39.75</v>
       </c>
-      <c r="H80" s="1">
-        <v>100</v>
-      </c>
-      <c r="I80" s="3">
-        <v>1891611.8556643024</v>
-      </c>
-      <c r="J80" s="3">
-        <v>2831538.3434146126</v>
-      </c>
-      <c r="K80" s="3">
-        <v>3116103.2433757163</v>
-      </c>
-      <c r="L80" s="3">
-        <v>7839253.4424546314</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>12</v>
       </c>
@@ -3573,23 +2337,8 @@
       <c r="G81" s="1">
         <v>32.869999999999997</v>
       </c>
-      <c r="H81" s="1">
-        <v>100</v>
-      </c>
-      <c r="I81" s="3">
-        <v>716034.15633552906</v>
-      </c>
-      <c r="J81" s="3">
-        <v>304071.38090564386</v>
-      </c>
-      <c r="K81" s="3">
-        <v>499491.56873405859</v>
-      </c>
-      <c r="L81" s="3">
-        <v>1519597.1059752316</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="15.7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:7" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>12</v>
       </c>
@@ -3610,21 +2359,6 @@
       </c>
       <c r="G82" s="1">
         <v>38.729999999999997</v>
-      </c>
-      <c r="H82" s="1">
-        <v>100</v>
-      </c>
-      <c r="I82" s="3">
-        <v>2563413.0297484128</v>
-      </c>
-      <c r="J82" s="3">
-        <v>3143720.5579218357</v>
-      </c>
-      <c r="K82" s="3">
-        <v>3607593.9913574131</v>
-      </c>
-      <c r="L82" s="3">
-        <v>9314727.5790276621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>